<commit_message>
include 10N2O in standard curves for leak test / fix excel overwrite problems
</commit_message>
<xml_diff>
--- a/GC-Data-Raw-R/GC-Data-Rprocessed/GC-Runs-Summary-Info/GCRunSummary_20140606_Leak0.xlsx
+++ b/GC-Data-Raw-R/GC-Data-Rprocessed/GC-Runs-Summary-Info/GCRunSummary_20140606_Leak0.xlsx
@@ -660,275 +660,283 @@
         <v>3.0</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="s" s="2">
+    <row r="34">
+      <c r="A34" t="n" s="3">
+        <v>235.2689</v>
+      </c>
+      <c r="B34" t="n" s="3">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="2">
         <v>57</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="s" s="1">
+    <row r="37">
+      <c r="A37" t="s" s="1">
         <v>28</v>
       </c>
-      <c r="B36" t="s" s="1">
+      <c r="B37" t="s" s="1">
         <v>27</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n" s="3">
-        <v>65.8166625</v>
-      </c>
-      <c r="B37" t="n" s="3">
-        <v>600.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n" s="3">
-        <v>0.0</v>
+        <v>65.8166625</v>
       </c>
       <c r="B38" t="n" s="3">
-        <v>0.0</v>
+        <v>600.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="B39" t="n" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n" s="3">
         <v>287.24171249999995</v>
       </c>
-      <c r="B39" t="n" s="3">
+      <c r="B40" t="n" s="3">
         <v>3000.0</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="s" s="2">
+    <row r="42">
+      <c r="A42" t="s" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="s" s="1">
+    <row r="43">
+      <c r="A43" t="s" s="1">
         <v>29</v>
       </c>
-      <c r="B42" t="s" s="1">
+      <c r="B43" t="s" s="1">
         <v>27</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="B43" t="n" s="3">
-        <v>0.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n" s="3">
-        <v>7.418837500000002</v>
+        <v>0.0</v>
       </c>
       <c r="B44" t="n" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n" s="3">
+        <v>7.418837500000002</v>
+      </c>
+      <c r="B45" t="n" s="3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n" s="3">
         <v>16.375337500000004</v>
       </c>
-      <c r="B45" t="n" s="3">
+      <c r="B46" t="n" s="3">
         <v>1.7</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="s" s="2">
+    <row r="48">
+      <c r="A48" t="s" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="s" s="1">
+    <row r="49">
+      <c r="A49" t="s" s="1">
         <v>30</v>
       </c>
-      <c r="B48" t="s" s="1">
+      <c r="B49" t="s" s="1">
         <v>31</v>
       </c>
-      <c r="C48" t="s" s="1">
+      <c r="C49" t="s" s="1">
         <v>32</v>
       </c>
-      <c r="D48" t="s" s="1">
+      <c r="D49" t="s" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="n" s="3">
-        <v>-0.18586844574978056</v>
-      </c>
-      <c r="B49" t="n" s="3">
-        <v>0.04105757090206041</v>
-      </c>
-      <c r="C49" t="n" s="3">
-        <v>0.9967485172862075</v>
-      </c>
-      <c r="D49" t="n" s="3">
-        <v>0.9935076067122531</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s" s="2">
+    <row r="50">
+      <c r="A50" t="n" s="3">
+        <v>-0.2888040654416866</v>
+      </c>
+      <c r="B50" t="n" s="3">
+        <v>0.043610146070702245</v>
+      </c>
+      <c r="C50" t="n" s="3">
+        <v>0.9996553771438316</v>
+      </c>
+      <c r="D50" t="n" s="3">
+        <v>0.9993108730525762</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="s" s="1">
+    <row r="53">
+      <c r="A53" t="s" s="1">
         <v>34</v>
       </c>
-      <c r="B52" t="s" s="1">
+      <c r="B53" t="s" s="1">
         <v>35</v>
       </c>
-      <c r="C52" t="s" s="1">
+      <c r="C53" t="s" s="1">
         <v>36</v>
       </c>
-      <c r="D52" t="s" s="1">
+      <c r="D53" t="s" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="n" s="3">
+    <row r="54">
+      <c r="A54" t="n" s="3">
         <v>-0.0740047963969769</v>
       </c>
-      <c r="B53" t="n" s="3">
+      <c r="B54" t="n" s="3">
         <v>0.0358775582904301</v>
       </c>
-      <c r="C53" t="n" s="3">
+      <c r="C54" t="n" s="3">
         <v>1.0</v>
       </c>
-      <c r="D53" t="n" s="3">
+      <c r="D54" t="n" s="3">
         <v>1.0</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="s" s="2">
+    <row r="56">
+      <c r="A56" t="s" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="s" s="1">
+    <row r="57">
+      <c r="A57" t="s" s="1">
         <v>38</v>
       </c>
-      <c r="B56" t="s" s="1">
+      <c r="B57" t="s" s="1">
         <v>39</v>
       </c>
-      <c r="C56" t="s" s="1">
+      <c r="C57" t="s" s="1">
         <v>40</v>
       </c>
-      <c r="D56" t="s" s="1">
+      <c r="D57" t="s" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="n" s="3">
+    <row r="58">
+      <c r="A58" t="n" s="3">
         <v>-40.913525673762464</v>
       </c>
-      <c r="B57" t="n" s="3">
+      <c r="B58" t="n" s="3">
         <v>10.544263613690761</v>
       </c>
-      <c r="C57" t="n" s="3">
+      <c r="C58" t="n" s="3">
         <v>0.9995397019658717</v>
       </c>
-      <c r="D57" t="n" s="3">
+      <c r="D58" t="n" s="3">
         <v>0.9990796158060237</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="s" s="2">
+    <row r="60">
+      <c r="A60" t="s" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="s" s="1">
+    <row r="61">
+      <c r="A61" t="s" s="1">
         <v>42</v>
       </c>
-      <c r="B60" t="s" s="1">
+      <c r="B61" t="s" s="1">
         <v>43</v>
       </c>
-      <c r="C60" t="s" s="1">
+      <c r="C61" t="s" s="1">
         <v>44</v>
       </c>
-      <c r="D60" t="s" s="1">
+      <c r="D61" t="s" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="n" s="3">
+    <row r="62">
+      <c r="A62" t="n" s="3">
         <v>-0.0</v>
       </c>
-      <c r="B61" t="n" s="3">
+      <c r="B62" t="n" s="3">
         <v>9.116232534580433</v>
       </c>
-      <c r="C61" t="n" s="3">
+      <c r="C62" t="n" s="3">
         <v>1.0</v>
       </c>
-      <c r="D61" t="n" s="3">
+      <c r="D62" t="n" s="3">
         <v>1.0</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="s" s="2">
+    <row r="64">
+      <c r="A64" t="s" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="s" s="1">
+    <row r="65">
+      <c r="A65" t="s" s="1">
         <v>46</v>
       </c>
-      <c r="B64" t="s" s="1">
+      <c r="B65" t="s" s="1">
         <v>47</v>
       </c>
-      <c r="C64" t="s" s="1">
+      <c r="C65" t="s" s="1">
         <v>48</v>
       </c>
-      <c r="D64" t="s" s="1">
+      <c r="D65" t="s" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="n" s="3">
+    <row r="66">
+      <c r="A66" t="n" s="3">
         <v>0.0835530675201405</v>
       </c>
-      <c r="B65" t="n" s="3">
+      <c r="B66" t="n" s="3">
         <v>0.10293867290795239</v>
       </c>
-      <c r="C65" t="n" s="3">
+      <c r="C66" t="n" s="3">
         <v>0.9879038751741666</v>
       </c>
-      <c r="D65" t="n" s="3">
+      <c r="D66" t="n" s="3">
         <v>0.9759540665841353</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" t="s" s="2">
+    <row r="68">
+      <c r="A68" t="s" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="s" s="1">
+    <row r="69">
+      <c r="A69" t="s" s="1">
         <v>50</v>
       </c>
-      <c r="B68" t="s" s="1">
+      <c r="B69" t="s" s="1">
         <v>51</v>
       </c>
-      <c r="C68" t="s" s="1">
+      <c r="C69" t="s" s="1">
         <v>52</v>
       </c>
-      <c r="D68" t="s" s="1">
+      <c r="D69" t="s" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" t="n" s="3">
+    <row r="70">
+      <c r="A70" t="n" s="3">
         <v>-0.0</v>
       </c>
-      <c r="B69" t="n" s="3">
+      <c r="B70" t="n" s="3">
         <v>0.13479200750791479</v>
       </c>
-      <c r="C69" t="n" s="3">
+      <c r="C70" t="n" s="3">
         <v>0.9999999999999999</v>
       </c>
-      <c r="D69" t="n" s="3">
+      <c r="D70" t="n" s="3">
         <v>0.9999999999999998</v>
       </c>
     </row>

</xml_diff>